<commit_message>
Anpassung an Formatrevision 2017
</commit_message>
<xml_diff>
--- a/VERZ_Importformat_HAN_Vorlage_20170517_bmt.xlsx
+++ b/VERZ_Importformat_HAN_Vorlage_20170517_bmt.xlsx
@@ -46,6 +46,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">Begriffslisten!$A$1:$D$117</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">Begriffslisten!$A$1:$D$117</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Begriffslisten!$A$1:$D$117</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">Begriffslisten!$A$1:$D$117</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -173,7 +174,7 @@
     <t xml:space="preserve">300e</t>
   </si>
   <si>
-    <t xml:space="preserve">500Aa</t>
+    <t xml:space="preserve">525a</t>
   </si>
   <si>
     <t xml:space="preserve">5441n</t>
@@ -512,7 +513,7 @@
     <t xml:space="preserve">260$c - z.B. : Ca. 1870-ca. 1890</t>
   </si>
   <si>
-    <t xml:space="preserve">008_Pos_07-14 / 593$a - z.B. 1870-1890</t>
+    <t xml:space="preserve">008_Pos_07-14 / 046$a$b$e - z.B. 1870-1890</t>
   </si>
   <si>
     <t xml:space="preserve">260$a</t>
@@ -560,7 +561,7 @@
     <t xml:space="preserve">300$e</t>
   </si>
   <si>
-    <t xml:space="preserve">500 A_ $a</t>
+    <t xml:space="preserve">525$a</t>
   </si>
   <si>
     <t xml:space="preserve">544 1_ $n</t>
@@ -575,10 +576,10 @@
     <t xml:space="preserve">533$n</t>
   </si>
   <si>
-    <t xml:space="preserve">856$u</t>
+    <t xml:space="preserve">856 _1 $u</t>
   </si>
   <si>
-    <t xml:space="preserve">856$z</t>
+    <t xml:space="preserve">856 _1 $z</t>
   </si>
   <si>
     <t xml:space="preserve">506$a</t>
@@ -1740,58 +1741,58 @@
   </sheetPr>
   <dimension ref="1:583"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z14" activeCellId="0" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.66964285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.45089285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="55.75"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="9.80357142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.1026785714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.7008928571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.0401785714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.44196428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.9375"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="51.0267857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.4107142857143"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.5535714285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.9910714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="18.8973214285714"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="22.4419642857143"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.7008928571429"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="14.0580357142857"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.6294642857143"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="13.2276785714286"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="10.0401785714286"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="13.7008928571429"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="18.5446428571429"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="28.2321428571429"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.5848214285714"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="11.1026785714286"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="12.5223214285714"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="10.8660714285714"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="11.1026785714286"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="23.3883928571429"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="10.9866071428571"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="11.1026785714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="12.0491071428571"/>
-    <col collapsed="false" hidden="false" max="50" min="41" style="1" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="1" width="25.9866071428571"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="1" width="23.03125"/>
-    <col collapsed="false" hidden="false" max="54" min="53" style="1" width="14.0580357142857"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="1" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="1" width="10.0401785714286"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="1" width="12.0491071428571"/>
-    <col collapsed="false" hidden="false" max="59" min="58" style="1" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="1022" min="60" style="1" width="9.92410714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="1" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.55357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.33035714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="55.0446428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.5848214285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.32142857142857"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="50.4375"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.1741071428571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.1964285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.7589285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="18.6607142857143"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="22.2053571428571"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.5848214285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.9910714285714"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="13.5848214285714"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="18.1919642857143"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="27.875"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="13.4642857142857"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="10.75"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="23.03125"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="10.8660714285714"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="11.8125"/>
+    <col collapsed="false" hidden="false" max="50" min="41" style="1" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="1" width="25.6294642857143"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="54" min="53" style="1" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="1" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="1" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="1" width="11.8125"/>
+    <col collapsed="false" hidden="false" max="59" min="58" style="1" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="1022" min="60" style="1" width="9.6875"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="1" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11594,7 +11595,7 @@
       <c r="AMI12" s="2"/>
       <c r="AMJ12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -47140,10 +47141,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="68" width="66.8526785714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="68" width="65.9107142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="68" width="9.21428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="68" width="9.92410714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="68" width="66.1473214285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="68" width="65.0848214285714"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="68" width="9.09375"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="68" width="9.6875"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48016,11 +48017,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="74" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="74" width="46.1830357142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="74" width="38.625"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="74" width="14.7633928571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="74" width="9.92410714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="74" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="74" width="45.59375"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="74" width="38.1517857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="74" width="14.5267857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="74" width="9.6875"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>